<commit_message>
Add code to get all team game logs.
</commit_message>
<xml_diff>
--- a/WNBA Table Columns.xlsx
+++ b/WNBA Table Columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Programming Projects (GitHub)\My Projects\wnba-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tg715c\Documents\Python Scripts\wnba-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BA2B9D3C-6DBE-4211-AE65-689C0C6B5D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A0C92E-4FDD-495F-9920-FEF4EEFF7FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1110" windowWidth="23085" windowHeight="12525" activeTab="6"/>
+    <workbookView xWindow="2325" yWindow="915" windowWidth="23295" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common_team_roster" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,49 @@
     <sheet name="players" sheetId="5" r:id="rId5"/>
     <sheet name="season_totals_regular_season" sheetId="6" r:id="rId6"/>
     <sheet name="teams" sheetId="7" r:id="rId7"/>
+    <sheet name="team_game_logs" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="166">
   <si>
     <t>TeamID</t>
   </si>
@@ -353,13 +389,184 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>1: "TEAM_ID"</t>
+  </si>
+  <si>
+    <t>2: "TEAM_ABBREVIATION"</t>
+  </si>
+  <si>
+    <t>3: "TEAM_NAME"</t>
+  </si>
+  <si>
+    <t>4: "GAME_ID"</t>
+  </si>
+  <si>
+    <t>5: "GAME_DATE"</t>
+  </si>
+  <si>
+    <t>6: "MATCHUP"</t>
+  </si>
+  <si>
+    <t>7: "WL"</t>
+  </si>
+  <si>
+    <t>8: "MIN"</t>
+  </si>
+  <si>
+    <t>9: "FGM"</t>
+  </si>
+  <si>
+    <t>10: "FGA"</t>
+  </si>
+  <si>
+    <t>11: "FG_PCT"</t>
+  </si>
+  <si>
+    <t>12: "FG3M"</t>
+  </si>
+  <si>
+    <t>13: "FG3A"</t>
+  </si>
+  <si>
+    <t>14: "FG3_PCT"</t>
+  </si>
+  <si>
+    <t>15: "FTM"</t>
+  </si>
+  <si>
+    <t>16: "FTA"</t>
+  </si>
+  <si>
+    <t>17: "FT_PCT"</t>
+  </si>
+  <si>
+    <t>18: "OREB"</t>
+  </si>
+  <si>
+    <t>19: "DREB"</t>
+  </si>
+  <si>
+    <t>20: "REB"</t>
+  </si>
+  <si>
+    <t>21: "AST"</t>
+  </si>
+  <si>
+    <t>22: "TOV"</t>
+  </si>
+  <si>
+    <t>23: "STL"</t>
+  </si>
+  <si>
+    <t>24: "BLK"</t>
+  </si>
+  <si>
+    <t>25: "BLKA"</t>
+  </si>
+  <si>
+    <t>26: "PF"</t>
+  </si>
+  <si>
+    <t>27: "PFD"</t>
+  </si>
+  <si>
+    <t>28: "PTS"</t>
+  </si>
+  <si>
+    <t>29: "PLUS_MINUS"</t>
+  </si>
+  <si>
+    <t>30: "GP_RANK"</t>
+  </si>
+  <si>
+    <t>31: "W_RANK"</t>
+  </si>
+  <si>
+    <t>32: "L_RANK"</t>
+  </si>
+  <si>
+    <t>33: "W_PCT_RANK"</t>
+  </si>
+  <si>
+    <t>34: "MIN_RANK"</t>
+  </si>
+  <si>
+    <t>35: "FGM_RANK"</t>
+  </si>
+  <si>
+    <t>36: "FGA_RANK"</t>
+  </si>
+  <si>
+    <t>37: "FG_PCT_RANK"</t>
+  </si>
+  <si>
+    <t>38: "FG3M_RANK"</t>
+  </si>
+  <si>
+    <t>39: "FG3A_RANK"</t>
+  </si>
+  <si>
+    <t>40: "FG3_PCT_RANK"</t>
+  </si>
+  <si>
+    <t>41: "FTM_RANK"</t>
+  </si>
+  <si>
+    <t>42: "FTA_RANK"</t>
+  </si>
+  <si>
+    <t>43: "FT_PCT_RANK"</t>
+  </si>
+  <si>
+    <t>44: "OREB_RANK"</t>
+  </si>
+  <si>
+    <t>45: "DREB_RANK"</t>
+  </si>
+  <si>
+    <t>46: "REB_RANK"</t>
+  </si>
+  <si>
+    <t>47: "AST_RANK"</t>
+  </si>
+  <si>
+    <t>48: "TOV_RANK"</t>
+  </si>
+  <si>
+    <t>49: "STL_RANK"</t>
+  </si>
+  <si>
+    <t>50: "BLK_RANK"</t>
+  </si>
+  <si>
+    <t>51: "BLKA_RANK"</t>
+  </si>
+  <si>
+    <t>52: "PF_RANK"</t>
+  </si>
+  <si>
+    <t>53: "PFD_RANK"</t>
+  </si>
+  <si>
+    <t>54: "PTS_RANK"</t>
+  </si>
+  <si>
+    <t>55: "PLUS_MINUS_RANK"</t>
+  </si>
+  <si>
+    <t>56: "AVAILABLE_FLAG"</t>
+  </si>
+  <si>
+    <t>0: "SEASON_YEAR"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1212,34 +1419,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1461,7 @@
         <v>"TeamID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1269,7 +1476,7 @@
         <v>"SEASON" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1284,7 +1491,7 @@
         <v>"LeagueID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1299,7 +1506,7 @@
         <v>"PLAYER" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1314,7 +1521,7 @@
         <v>"NICKNAME" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1536,7 @@
         <v>"PLAYER_SLUG" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1344,7 +1551,7 @@
         <v>"NUM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1359,7 +1566,7 @@
         <v>"POSITION" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1374,7 +1581,7 @@
         <v>"HEIGHT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1596,7 @@
         <v>"WEIGHT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1404,7 +1611,7 @@
         <v>"BIRTH_DATE" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1626,7 @@
         <v>"AGE" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1641,7 @@
         <v>"EXP" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1656,7 @@
         <v>"SCHOOL" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1464,7 +1671,7 @@
         <v>"PLAYER_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1485,22 +1692,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1515,7 +1722,7 @@
         <v>"date_generated" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1737,7 @@
         <v>"seasons_count" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1545,7 +1752,7 @@
         <v>"teams_count" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1566,22 +1773,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1596,7 +1803,7 @@
         <v>"PLAYER_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1611,7 +1818,7 @@
         <v>"SEASON_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1833,7 @@
         <v>"LEAGUE_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1641,7 +1848,7 @@
         <v>"TEAM_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1656,7 +1863,7 @@
         <v>"TEAM_ABBREVIATION" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1671,7 +1878,7 @@
         <v>"PLAYER_AGE" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1686,7 +1893,7 @@
         <v>"GP" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1701,7 +1908,7 @@
         <v>"GS" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1716,7 +1923,7 @@
         <v>"MIN" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1731,7 +1938,7 @@
         <v>"FGM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1746,7 +1953,7 @@
         <v>"FGA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1761,7 +1968,7 @@
         <v>"FG_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1776,7 +1983,7 @@
         <v>"FG3M" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1791,7 +1998,7 @@
         <v>"FG3A" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1806,7 +2013,7 @@
         <v>"FG3_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1821,7 +2028,7 @@
         <v>"FTM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1836,7 +2043,7 @@
         <v>"FTA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1851,7 +2058,7 @@
         <v>"FT_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1866,7 +2073,7 @@
         <v>"OREB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1881,7 +2088,7 @@
         <v>"DREB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1896,7 +2103,7 @@
         <v>"REB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1911,7 +2118,7 @@
         <v>"AST" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1926,7 +2133,7 @@
         <v>"STL" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1941,7 +2148,7 @@
         <v>"BLK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1956,7 +2163,7 @@
         <v>"TOV" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1971,7 +2178,7 @@
         <v>"PF" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1992,22 +2199,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2022,7 +2229,7 @@
         <v>"SEASON_YEAR" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2037,7 +2244,7 @@
         <v>"PLAYER_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2052,7 +2259,7 @@
         <v>"PLAYER_NAME" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2274,7 @@
         <v>"NICKNAME" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2082,7 +2289,7 @@
         <v>"TEAM_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2097,7 +2304,7 @@
         <v>"TEAM_ABBREVIATION" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2112,7 +2319,7 @@
         <v>"TEAM_NAME" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -2127,7 +2334,7 @@
         <v>"GAME_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2142,7 +2349,7 @@
         <v>"GAME_DATE" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2157,7 +2364,7 @@
         <v>"MATCHUP" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2172,7 +2379,7 @@
         <v>"WL" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2187,7 +2394,7 @@
         <v>"MIN" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2202,7 +2409,7 @@
         <v>"FGM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2217,7 +2424,7 @@
         <v>"FGA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2232,7 +2439,7 @@
         <v>"FG_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2247,7 +2454,7 @@
         <v>"FG3M" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2262,7 +2469,7 @@
         <v>"FG3A" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2277,7 +2484,7 @@
         <v>"FG3_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2292,7 +2499,7 @@
         <v>"FTM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2307,7 +2514,7 @@
         <v>"FTA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -2322,7 +2529,7 @@
         <v>"FT_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2337,7 +2544,7 @@
         <v>"OREB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2352,7 +2559,7 @@
         <v>"DREB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2367,7 +2574,7 @@
         <v>"REB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2382,7 +2589,7 @@
         <v>"AST" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -2397,7 +2604,7 @@
         <v>"TOV" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2619,7 @@
         <v>"STL" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2427,7 +2634,7 @@
         <v>"BLK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -2442,7 +2649,7 @@
         <v>"BLKA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2457,7 +2664,7 @@
         <v>"PF" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -2472,7 +2679,7 @@
         <v>"PFD" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2487,7 +2694,7 @@
         <v>"PTS" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -2502,7 +2709,7 @@
         <v>"PLUS_MINUS" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2517,7 +2724,7 @@
         <v>"NBA_FANTASY_PTS" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -2532,7 +2739,7 @@
         <v>"DD2" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2547,7 +2754,7 @@
         <v>"TD3" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -2562,7 +2769,7 @@
         <v>"WNBA_FANTASY_PTS" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -2577,7 +2784,7 @@
         <v>"GP_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -2592,7 +2799,7 @@
         <v>"W_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -2607,7 +2814,7 @@
         <v>"L_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -2622,7 +2829,7 @@
         <v>"W_PCT_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -2637,7 +2844,7 @@
         <v>"MIN_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -2652,7 +2859,7 @@
         <v>"FGM_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -2667,7 +2874,7 @@
         <v>"FGA_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -2682,7 +2889,7 @@
         <v>"FG_PCT_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -2697,7 +2904,7 @@
         <v>"FG3M_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -2712,7 +2919,7 @@
         <v>"FG3A_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2727,7 +2934,7 @@
         <v>"FG3_PCT_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -2742,7 +2949,7 @@
         <v>"FTM_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -2757,7 +2964,7 @@
         <v>"FTA_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -2772,7 +2979,7 @@
         <v>"FT_PCT_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -2787,7 +2994,7 @@
         <v>"OREB_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>77</v>
       </c>
@@ -2802,7 +3009,7 @@
         <v>"DREB_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2817,7 +3024,7 @@
         <v>"REB_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -2832,7 +3039,7 @@
         <v>"AST_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -2847,7 +3054,7 @@
         <v>"TOV_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>81</v>
       </c>
@@ -2862,7 +3069,7 @@
         <v>"STL_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -2877,7 +3084,7 @@
         <v>"BLK_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -2892,7 +3099,7 @@
         <v>"BLKA_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>84</v>
       </c>
@@ -2907,7 +3114,7 @@
         <v>"PF_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -2922,7 +3129,7 @@
         <v>"PFD_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -2937,7 +3144,7 @@
         <v>"PTS_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>87</v>
       </c>
@@ -2952,7 +3159,7 @@
         <v>"PLUS_MINUS_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2967,7 +3174,7 @@
         <v>"NBA_FANTASY_PTS_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>89</v>
       </c>
@@ -2982,7 +3189,7 @@
         <v>"DD2_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -2997,7 +3204,7 @@
         <v>"TD3_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>91</v>
       </c>
@@ -3012,7 +3219,7 @@
         <v>"WNBA_FANTASY_PTS_RANK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>92</v>
       </c>
@@ -3033,22 +3240,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -3063,7 +3270,7 @@
         <v>"player_id" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -3078,7 +3285,7 @@
         <v>"player_name" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -3093,7 +3300,7 @@
         <v>"active_flag" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -3108,7 +3315,7 @@
         <v>"rookie_season" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -3123,7 +3330,7 @@
         <v>"last_season" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -3138,7 +3345,7 @@
         <v>"unknown" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -3159,22 +3366,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3189,7 +3396,7 @@
         <v>"PLAYER_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3204,7 +3411,7 @@
         <v>"SEASON_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3219,7 +3426,7 @@
         <v>"LEAGUE_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3441,7 @@
         <v>"TEAM_ID" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3249,7 +3456,7 @@
         <v>"TEAM_ABBREVIATION" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3264,7 +3471,7 @@
         <v>"PLAYER_AGE" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3279,7 +3486,7 @@
         <v>"GP" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -3294,7 +3501,7 @@
         <v>"GS" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3309,7 +3516,7 @@
         <v>"MIN" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -3324,7 +3531,7 @@
         <v>"FGM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3339,7 +3546,7 @@
         <v>"FGA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -3354,7 +3561,7 @@
         <v>"FG_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3369,7 +3576,7 @@
         <v>"FG3M" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -3384,7 +3591,7 @@
         <v>"FG3A" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3399,7 +3606,7 @@
         <v>"FG3_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3414,7 +3621,7 @@
         <v>"FTM" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -3429,7 +3636,7 @@
         <v>"FTA" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3444,7 +3651,7 @@
         <v>"FT_PCT" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3459,7 +3666,7 @@
         <v>"OREB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3474,7 +3681,7 @@
         <v>"DREB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -3489,7 +3696,7 @@
         <v>"REB" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -3504,7 +3711,7 @@
         <v>"AST" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -3519,7 +3726,7 @@
         <v>"STL" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3534,7 +3741,7 @@
         <v>"BLK" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3549,7 +3756,7 @@
         <v>"TOV" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3564,7 +3771,7 @@
         <v>"PF" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3585,22 +3792,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -3615,7 +3822,7 @@
         <v>"team_id" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -3630,7 +3837,7 @@
         <v>"team_abbreviation" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3645,7 +3852,7 @@
         <v>"team_name" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -3660,7 +3867,7 @@
         <v>"team_city" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -3675,7 +3882,7 @@
         <v>"team_state" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -3690,7 +3897,7 @@
         <v>"time_zone" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -3705,7 +3912,7 @@
         <v>"primary_color" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -3720,7 +3927,7 @@
         <v>"secondary_color" VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -3738,4 +3945,1509 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F8D3D1-9A33-4874-9CEA-68E5282DA8C2}">
+  <dimension ref="A2:H58"/>
+  <sheetViews>
+    <sheetView topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:C2">_xlfn.TEXTSPLIT(A2, ":")</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v xml:space="preserve"> "SEASON_YEAR"</v>
+      </c>
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(C2, CHAR(34), )</f>
+        <v xml:space="preserve"> SEASON_YEAR</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(D2," ",E2," ", F2, CHAR(44))</f>
+        <v xml:space="preserve"> SEASON_YEAR VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3:C3">_xlfn.TEXTSPLIT(A3, ":")</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve"> "TEAM_ID"</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D58" si="0">SUBSTITUTE(C3, CHAR(34), )</f>
+        <v xml:space="preserve"> TEAM_ID</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H58" si="1">CONCATENATE(D3," ",E3," ", F3, CHAR(44))</f>
+        <v xml:space="preserve"> TEAM_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4:C4">_xlfn.TEXTSPLIT(A4, ":")</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="str">
+        <v xml:space="preserve"> "TEAM_ABBREVIATION"</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_ABBREVIATION</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> TEAM_ABBREVIATION VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5:C5">_xlfn.TEXTSPLIT(A5, ":")</f>
+        <v>3</v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve"> "TEAM_NAME"</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_NAME</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> TEAM_NAME VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6:C6">_xlfn.TEXTSPLIT(A6, ":")</f>
+        <v>4</v>
+      </c>
+      <c r="C6" t="str">
+        <v xml:space="preserve"> "GAME_ID"</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> GAME_ID</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> GAME_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="str" cm="1">
+        <f t="array" ref="B7:C7">_xlfn.TEXTSPLIT(A7, ":")</f>
+        <v>5</v>
+      </c>
+      <c r="C7" t="str">
+        <v xml:space="preserve"> "GAME_DATE"</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> GAME_DATE</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> GAME_DATE VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="str" cm="1">
+        <f t="array" ref="B8:C8">_xlfn.TEXTSPLIT(A8, ":")</f>
+        <v>6</v>
+      </c>
+      <c r="C8" t="str">
+        <v xml:space="preserve"> "MATCHUP"</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> MATCHUP</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> MATCHUP VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="str" cm="1">
+        <f t="array" ref="B9:C9">_xlfn.TEXTSPLIT(A9, ":")</f>
+        <v>7</v>
+      </c>
+      <c r="C9" t="str">
+        <v xml:space="preserve"> "WL"</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> WL</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> WL VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:C10">_xlfn.TEXTSPLIT(A10, ":")</f>
+        <v>8</v>
+      </c>
+      <c r="C10" t="str">
+        <v xml:space="preserve"> "MIN"</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> MIN</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> MIN VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="str" cm="1">
+        <f t="array" ref="B11:C11">_xlfn.TEXTSPLIT(A11, ":")</f>
+        <v>9</v>
+      </c>
+      <c r="C11" t="str">
+        <v xml:space="preserve"> "FGM"</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGM</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FGM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="str" cm="1">
+        <f t="array" ref="B12:C12">_xlfn.TEXTSPLIT(A12, ":")</f>
+        <v>10</v>
+      </c>
+      <c r="C12" t="str">
+        <v xml:space="preserve"> "FGA"</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGA</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FGA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="str" cm="1">
+        <f t="array" ref="B13:C13">_xlfn.TEXTSPLIT(A13, ":")</f>
+        <v>11</v>
+      </c>
+      <c r="C13" t="str">
+        <v xml:space="preserve"> "FG_PCT"</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG_PCT</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="str" cm="1">
+        <f t="array" ref="B14:C14">_xlfn.TEXTSPLIT(A14, ":")</f>
+        <v>12</v>
+      </c>
+      <c r="C14" t="str">
+        <v xml:space="preserve"> "FG3M"</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3M</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG3M VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15:C15">_xlfn.TEXTSPLIT(A15, ":")</f>
+        <v>13</v>
+      </c>
+      <c r="C15" t="str">
+        <v xml:space="preserve"> "FG3A"</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3A</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG3A VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="str" cm="1">
+        <f t="array" ref="B16:C16">_xlfn.TEXTSPLIT(A16, ":")</f>
+        <v>14</v>
+      </c>
+      <c r="C16" t="str">
+        <v xml:space="preserve"> "FG3_PCT"</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3_PCT</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG3_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="str" cm="1">
+        <f t="array" ref="B17:C17">_xlfn.TEXTSPLIT(A17, ":")</f>
+        <v>15</v>
+      </c>
+      <c r="C17" t="str">
+        <v xml:space="preserve"> "FTM"</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTM</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FTM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="str" cm="1">
+        <f t="array" ref="B18:C18">_xlfn.TEXTSPLIT(A18, ":")</f>
+        <v>16</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve"> "FTA"</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTA</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FTA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="str" cm="1">
+        <f t="array" ref="B19:C19">_xlfn.TEXTSPLIT(A19, ":")</f>
+        <v>17</v>
+      </c>
+      <c r="C19" t="str">
+        <v xml:space="preserve"> "FT_PCT"</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FT_PCT</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FT_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="str" cm="1">
+        <f t="array" ref="B20:C20">_xlfn.TEXTSPLIT(A20, ":")</f>
+        <v>18</v>
+      </c>
+      <c r="C20" t="str">
+        <v xml:space="preserve"> "OREB"</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> OREB</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> OREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="str" cm="1">
+        <f t="array" ref="B21:C21">_xlfn.TEXTSPLIT(A21, ":")</f>
+        <v>19</v>
+      </c>
+      <c r="C21" t="str">
+        <v xml:space="preserve"> "DREB"</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> DREB</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> DREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="str" cm="1">
+        <f t="array" ref="B22:C22">_xlfn.TEXTSPLIT(A22, ":")</f>
+        <v>20</v>
+      </c>
+      <c r="C22" t="str">
+        <v xml:space="preserve"> "REB"</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> REB</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> REB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="str" cm="1">
+        <f t="array" ref="B23:C23">_xlfn.TEXTSPLIT(A23, ":")</f>
+        <v>21</v>
+      </c>
+      <c r="C23" t="str">
+        <v xml:space="preserve"> "AST"</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> AST</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> AST VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="str" cm="1">
+        <f t="array" ref="B24:C24">_xlfn.TEXTSPLIT(A24, ":")</f>
+        <v>22</v>
+      </c>
+      <c r="C24" t="str">
+        <v xml:space="preserve"> "TOV"</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TOV</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> TOV VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" t="str" cm="1">
+        <f t="array" ref="B25:C25">_xlfn.TEXTSPLIT(A25, ":")</f>
+        <v>23</v>
+      </c>
+      <c r="C25" t="str">
+        <v xml:space="preserve"> "STL"</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> STL</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> STL VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="str" cm="1">
+        <f t="array" ref="B26:C26">_xlfn.TEXTSPLIT(A26, ":")</f>
+        <v>24</v>
+      </c>
+      <c r="C26" t="str">
+        <v xml:space="preserve"> "BLK"</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLK</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> BLK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" t="str" cm="1">
+        <f t="array" ref="B27:C27">_xlfn.TEXTSPLIT(A27, ":")</f>
+        <v>25</v>
+      </c>
+      <c r="C27" t="str">
+        <v xml:space="preserve"> "BLKA"</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLKA</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> BLKA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="str" cm="1">
+        <f t="array" ref="B28:C28">_xlfn.TEXTSPLIT(A28, ":")</f>
+        <v>26</v>
+      </c>
+      <c r="C28" t="str">
+        <v xml:space="preserve"> "PF"</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PF</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PF VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="str" cm="1">
+        <f t="array" ref="B29:C29">_xlfn.TEXTSPLIT(A29, ":")</f>
+        <v>27</v>
+      </c>
+      <c r="C29" t="str">
+        <v xml:space="preserve"> "PFD"</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PFD</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PFD VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="str" cm="1">
+        <f t="array" ref="B30:C30">_xlfn.TEXTSPLIT(A30, ":")</f>
+        <v>28</v>
+      </c>
+      <c r="C30" t="str">
+        <v xml:space="preserve"> "PTS"</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PTS</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PTS VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" t="str" cm="1">
+        <f t="array" ref="B31:C31">_xlfn.TEXTSPLIT(A31, ":")</f>
+        <v>29</v>
+      </c>
+      <c r="C31" t="str">
+        <v xml:space="preserve"> "PLUS_MINUS"</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PLUS_MINUS</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PLUS_MINUS VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="str" cm="1">
+        <f t="array" ref="B32:C32">_xlfn.TEXTSPLIT(A32, ":")</f>
+        <v>30</v>
+      </c>
+      <c r="C32" t="str">
+        <v xml:space="preserve"> "GP_RANK"</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> GP_RANK</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> GP_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" t="str" cm="1">
+        <f t="array" ref="B33:C33">_xlfn.TEXTSPLIT(A33, ":")</f>
+        <v>31</v>
+      </c>
+      <c r="C33" t="str">
+        <v xml:space="preserve"> "W_RANK"</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> W_RANK</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> W_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" t="str" cm="1">
+        <f t="array" ref="B34:C34">_xlfn.TEXTSPLIT(A34, ":")</f>
+        <v>32</v>
+      </c>
+      <c r="C34" t="str">
+        <v xml:space="preserve"> "L_RANK"</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> L_RANK</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> L_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" t="str" cm="1">
+        <f t="array" ref="B35:C35">_xlfn.TEXTSPLIT(A35, ":")</f>
+        <v>33</v>
+      </c>
+      <c r="C35" t="str">
+        <v xml:space="preserve"> "W_PCT_RANK"</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> W_PCT_RANK</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> W_PCT_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="str" cm="1">
+        <f t="array" ref="B36:C36">_xlfn.TEXTSPLIT(A36, ":")</f>
+        <v>34</v>
+      </c>
+      <c r="C36" t="str">
+        <v xml:space="preserve"> "MIN_RANK"</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> MIN_RANK</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> MIN_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" t="str" cm="1">
+        <f t="array" ref="B37:C37">_xlfn.TEXTSPLIT(A37, ":")</f>
+        <v>35</v>
+      </c>
+      <c r="C37" t="str">
+        <v xml:space="preserve"> "FGM_RANK"</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGM_RANK</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FGM_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" t="str" cm="1">
+        <f t="array" ref="B38:C38">_xlfn.TEXTSPLIT(A38, ":")</f>
+        <v>36</v>
+      </c>
+      <c r="C38" t="str">
+        <v xml:space="preserve"> "FGA_RANK"</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGA_RANK</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FGA_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" t="str" cm="1">
+        <f t="array" ref="B39:C39">_xlfn.TEXTSPLIT(A39, ":")</f>
+        <v>37</v>
+      </c>
+      <c r="C39" t="str">
+        <v xml:space="preserve"> "FG_PCT_RANK"</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG_PCT_RANK</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG_PCT_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" t="str" cm="1">
+        <f t="array" ref="B40:C40">_xlfn.TEXTSPLIT(A40, ":")</f>
+        <v>38</v>
+      </c>
+      <c r="C40" t="str">
+        <v xml:space="preserve"> "FG3M_RANK"</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3M_RANK</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG3M_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" t="str" cm="1">
+        <f t="array" ref="B41:C41">_xlfn.TEXTSPLIT(A41, ":")</f>
+        <v>39</v>
+      </c>
+      <c r="C41" t="str">
+        <v xml:space="preserve"> "FG3A_RANK"</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3A_RANK</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG3A_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" t="str" cm="1">
+        <f t="array" ref="B42:C42">_xlfn.TEXTSPLIT(A42, ":")</f>
+        <v>40</v>
+      </c>
+      <c r="C42" t="str">
+        <v xml:space="preserve"> "FG3_PCT_RANK"</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3_PCT_RANK</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FG3_PCT_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" t="str" cm="1">
+        <f t="array" ref="B43:C43">_xlfn.TEXTSPLIT(A43, ":")</f>
+        <v>41</v>
+      </c>
+      <c r="C43" t="str">
+        <v xml:space="preserve"> "FTM_RANK"</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTM_RANK</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FTM_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" t="str" cm="1">
+        <f t="array" ref="B44:C44">_xlfn.TEXTSPLIT(A44, ":")</f>
+        <v>42</v>
+      </c>
+      <c r="C44" t="str">
+        <v xml:space="preserve"> "FTA_RANK"</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTA_RANK</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FTA_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" t="str" cm="1">
+        <f t="array" ref="B45:C45">_xlfn.TEXTSPLIT(A45, ":")</f>
+        <v>43</v>
+      </c>
+      <c r="C45" t="str">
+        <v xml:space="preserve"> "FT_PCT_RANK"</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FT_PCT_RANK</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> FT_PCT_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" t="str" cm="1">
+        <f t="array" ref="B46:C46">_xlfn.TEXTSPLIT(A46, ":")</f>
+        <v>44</v>
+      </c>
+      <c r="C46" t="str">
+        <v xml:space="preserve"> "OREB_RANK"</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> OREB_RANK</v>
+      </c>
+      <c r="E46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> OREB_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" t="str" cm="1">
+        <f t="array" ref="B47:C47">_xlfn.TEXTSPLIT(A47, ":")</f>
+        <v>45</v>
+      </c>
+      <c r="C47" t="str">
+        <v xml:space="preserve"> "DREB_RANK"</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> DREB_RANK</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> DREB_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" t="str" cm="1">
+        <f t="array" ref="B48:C48">_xlfn.TEXTSPLIT(A48, ":")</f>
+        <v>46</v>
+      </c>
+      <c r="C48" t="str">
+        <v xml:space="preserve"> "REB_RANK"</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> REB_RANK</v>
+      </c>
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> REB_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" t="str" cm="1">
+        <f t="array" ref="B49:C49">_xlfn.TEXTSPLIT(A49, ":")</f>
+        <v>47</v>
+      </c>
+      <c r="C49" t="str">
+        <v xml:space="preserve"> "AST_RANK"</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> AST_RANK</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> AST_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" t="str" cm="1">
+        <f t="array" ref="B50:C50">_xlfn.TEXTSPLIT(A50, ":")</f>
+        <v>48</v>
+      </c>
+      <c r="C50" t="str">
+        <v xml:space="preserve"> "TOV_RANK"</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TOV_RANK</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> TOV_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" t="str" cm="1">
+        <f t="array" ref="B51:C51">_xlfn.TEXTSPLIT(A51, ":")</f>
+        <v>49</v>
+      </c>
+      <c r="C51" t="str">
+        <v xml:space="preserve"> "STL_RANK"</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> STL_RANK</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> STL_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" t="str" cm="1">
+        <f t="array" ref="B52:C52">_xlfn.TEXTSPLIT(A52, ":")</f>
+        <v>50</v>
+      </c>
+      <c r="C52" t="str">
+        <v xml:space="preserve"> "BLK_RANK"</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLK_RANK</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> BLK_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" t="str" cm="1">
+        <f t="array" ref="B53:C53">_xlfn.TEXTSPLIT(A53, ":")</f>
+        <v>51</v>
+      </c>
+      <c r="C53" t="str">
+        <v xml:space="preserve"> "BLKA_RANK"</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLKA_RANK</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> BLKA_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" t="str" cm="1">
+        <f t="array" ref="B54:C54">_xlfn.TEXTSPLIT(A54, ":")</f>
+        <v>52</v>
+      </c>
+      <c r="C54" t="str">
+        <v xml:space="preserve"> "PF_RANK"</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PF_RANK</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PF_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" t="str" cm="1">
+        <f t="array" ref="B55:C55">_xlfn.TEXTSPLIT(A55, ":")</f>
+        <v>53</v>
+      </c>
+      <c r="C55" t="str">
+        <v xml:space="preserve"> "PFD_RANK"</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PFD_RANK</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PFD_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" t="str" cm="1">
+        <f t="array" ref="B56:C56">_xlfn.TEXTSPLIT(A56, ":")</f>
+        <v>54</v>
+      </c>
+      <c r="C56" t="str">
+        <v xml:space="preserve"> "PTS_RANK"</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PTS_RANK</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PTS_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" t="str" cm="1">
+        <f t="array" ref="B57:C57">_xlfn.TEXTSPLIT(A57, ":")</f>
+        <v>55</v>
+      </c>
+      <c r="C57" t="str">
+        <v xml:space="preserve"> "PLUS_MINUS_RANK"</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PLUS_MINUS_RANK</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> PLUS_MINUS_RANK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" t="str" cm="1">
+        <f t="array" ref="B58:C58">_xlfn.TEXTSPLIT(A58, ":")</f>
+        <v>56</v>
+      </c>
+      <c r="C58" t="str">
+        <v xml:space="preserve"> "AVAILABLE_FLAG"</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> AVAILABLE_FLAG</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> AVAILABLE_FLAG VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add code to save all game logs to database.
</commit_message>
<xml_diff>
--- a/WNBA Table Columns.xlsx
+++ b/WNBA Table Columns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tg715c\Documents\Python Scripts\wnba-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A0C92E-4FDD-495F-9920-FEF4EEFF7FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259F4E92-4196-4238-B2FD-22C402FDF6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="915" windowWidth="23295" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="1200" windowWidth="23295" windowHeight="13035" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common_team_roster" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="season_totals_regular_season" sheetId="6" r:id="rId6"/>
     <sheet name="teams" sheetId="7" r:id="rId7"/>
     <sheet name="team_game_logs" sheetId="8" r:id="rId8"/>
+    <sheet name="boxscore_player_stats" sheetId="9" r:id="rId9"/>
+    <sheet name="boxscore_team_stats" sheetId="10" r:id="rId10"/>
+    <sheet name="boxscore_team_start_bench_stats" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="233">
   <si>
     <t>TeamID</t>
   </si>
@@ -560,6 +563,207 @@
   </si>
   <si>
     <t>0: "SEASON_YEAR"</t>
+  </si>
+  <si>
+    <t>0: "GAME_ID"</t>
+  </si>
+  <si>
+    <t>3: "TEAM_CITY"</t>
+  </si>
+  <si>
+    <t>4: "PLAYER_ID"</t>
+  </si>
+  <si>
+    <t>5: "PLAYER_NAME"</t>
+  </si>
+  <si>
+    <t>6: "NICKNAME"</t>
+  </si>
+  <si>
+    <t>7: "START_POSITION"</t>
+  </si>
+  <si>
+    <t>8: "COMMENT"</t>
+  </si>
+  <si>
+    <t>9: "MIN"</t>
+  </si>
+  <si>
+    <t>10: "FGM"</t>
+  </si>
+  <si>
+    <t>11: "FGA"</t>
+  </si>
+  <si>
+    <t>12: "FG_PCT"</t>
+  </si>
+  <si>
+    <t>13: "FG3M"</t>
+  </si>
+  <si>
+    <t>14: "FG3A"</t>
+  </si>
+  <si>
+    <t>15: "FG3_PCT"</t>
+  </si>
+  <si>
+    <t>16: "FTM"</t>
+  </si>
+  <si>
+    <t>17: "FTA"</t>
+  </si>
+  <si>
+    <t>18: "FT_PCT"</t>
+  </si>
+  <si>
+    <t>19: "OREB"</t>
+  </si>
+  <si>
+    <t>20: "DREB"</t>
+  </si>
+  <si>
+    <t>21: "REB"</t>
+  </si>
+  <si>
+    <t>22: "AST"</t>
+  </si>
+  <si>
+    <t>25: "TO"</t>
+  </si>
+  <si>
+    <t>27: "PTS"</t>
+  </si>
+  <si>
+    <t>28: "PLUS_MINUS"</t>
+  </si>
+  <si>
+    <t>2: "TEAM_NAME"</t>
+  </si>
+  <si>
+    <t>3: "TEAM_ABBREVIATION"</t>
+  </si>
+  <si>
+    <t>4: "TEAM_CITY"</t>
+  </si>
+  <si>
+    <t>5: "MIN"</t>
+  </si>
+  <si>
+    <t>6: "FGM"</t>
+  </si>
+  <si>
+    <t>7: "FGA"</t>
+  </si>
+  <si>
+    <t>8: "FG_PCT"</t>
+  </si>
+  <si>
+    <t>9: "FG3M"</t>
+  </si>
+  <si>
+    <t>10: "FG3A"</t>
+  </si>
+  <si>
+    <t>11: "FG3_PCT"</t>
+  </si>
+  <si>
+    <t>12: "FTM"</t>
+  </si>
+  <si>
+    <t>13: "FTA"</t>
+  </si>
+  <si>
+    <t>14: "FT_PCT"</t>
+  </si>
+  <si>
+    <t>15: "OREB"</t>
+  </si>
+  <si>
+    <t>16: "DREB"</t>
+  </si>
+  <si>
+    <t>17: "REB"</t>
+  </si>
+  <si>
+    <t>18: "AST"</t>
+  </si>
+  <si>
+    <t>19: "STL"</t>
+  </si>
+  <si>
+    <t>20: "BLK"</t>
+  </si>
+  <si>
+    <t>21: "TO"</t>
+  </si>
+  <si>
+    <t>22: "PF"</t>
+  </si>
+  <si>
+    <t>23: "PTS"</t>
+  </si>
+  <si>
+    <t>24: "PLUS_MINUS"</t>
+  </si>
+  <si>
+    <t>5: "STARTERS_BENCH"</t>
+  </si>
+  <si>
+    <t>6: "MIN"</t>
+  </si>
+  <si>
+    <t>7: "FGM"</t>
+  </si>
+  <si>
+    <t>8: "FGA"</t>
+  </si>
+  <si>
+    <t>9: "FG_PCT"</t>
+  </si>
+  <si>
+    <t>10: "FG3M"</t>
+  </si>
+  <si>
+    <t>11: "FG3A"</t>
+  </si>
+  <si>
+    <t>12: "FG3_PCT"</t>
+  </si>
+  <si>
+    <t>13: "FTM"</t>
+  </si>
+  <si>
+    <t>14: "FTA"</t>
+  </si>
+  <si>
+    <t>15: "FT_PCT"</t>
+  </si>
+  <si>
+    <t>16: "OREB"</t>
+  </si>
+  <si>
+    <t>17: "DREB"</t>
+  </si>
+  <si>
+    <t>18: "REB"</t>
+  </si>
+  <si>
+    <t>19: "AST"</t>
+  </si>
+  <si>
+    <t>20: "STL"</t>
+  </si>
+  <si>
+    <t>21: "BLK"</t>
+  </si>
+  <si>
+    <t>22: "TO"</t>
+  </si>
+  <si>
+    <t>23: "PF"</t>
+  </si>
+  <si>
+    <t>24: "PTS"</t>
   </si>
 </sst>
 </file>
@@ -1691,6 +1895,1354 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0424CE45-272A-4D2A-96EE-F0448F9E2485}">
+  <dimension ref="A2:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:C2">_xlfn.TEXTSPLIT(A2, ":")</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v xml:space="preserve"> "GAME_ID"</v>
+      </c>
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(C2, CHAR(34), )</f>
+        <v xml:space="preserve"> GAME_ID</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(TRIM(D2)," ",E2," ", F2, CHAR(44))</f>
+        <v>GAME_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3:C3">_xlfn.TEXTSPLIT(A3, ":")</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve"> "TEAM_ID"</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">SUBSTITUTE(C3, CHAR(34), )</f>
+        <v xml:space="preserve"> TEAM_ID</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H26" si="1">CONCATENATE(TRIM(D3)," ",E3," ", F3, CHAR(44))</f>
+        <v>TEAM_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4:C4">_xlfn.TEXTSPLIT(A4, ":")</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="str">
+        <v xml:space="preserve"> "TEAM_NAME"</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_NAME</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_NAME VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5:C5">_xlfn.TEXTSPLIT(A5, ":")</f>
+        <v>3</v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve"> "TEAM_ABBREVIATION"</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_ABBREVIATION</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_ABBREVIATION VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6:C6">_xlfn.TEXTSPLIT(A6, ":")</f>
+        <v>4</v>
+      </c>
+      <c r="C6" t="str">
+        <v xml:space="preserve"> "TEAM_CITY"</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_CITY</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_CITY VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" t="str" cm="1">
+        <f t="array" ref="B7:C7">_xlfn.TEXTSPLIT(A7, ":")</f>
+        <v>5</v>
+      </c>
+      <c r="C7" t="str">
+        <v xml:space="preserve"> "MIN"</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> MIN</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>MIN VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" t="str" cm="1">
+        <f t="array" ref="B8:C8">_xlfn.TEXTSPLIT(A8, ":")</f>
+        <v>6</v>
+      </c>
+      <c r="C8" t="str">
+        <v xml:space="preserve"> "FGM"</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGM</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>FGM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" t="str" cm="1">
+        <f t="array" ref="B9:C9">_xlfn.TEXTSPLIT(A9, ":")</f>
+        <v>7</v>
+      </c>
+      <c r="C9" t="str">
+        <v xml:space="preserve"> "FGA"</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGA</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>FGA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:C10">_xlfn.TEXTSPLIT(A10, ":")</f>
+        <v>8</v>
+      </c>
+      <c r="C10" t="str">
+        <v xml:space="preserve"> "FG_PCT"</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG_PCT</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>FG_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" t="str" cm="1">
+        <f t="array" ref="B11:C11">_xlfn.TEXTSPLIT(A11, ":")</f>
+        <v>9</v>
+      </c>
+      <c r="C11" t="str">
+        <v xml:space="preserve"> "FG3M"</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3M</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3M VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" t="str" cm="1">
+        <f t="array" ref="B12:C12">_xlfn.TEXTSPLIT(A12, ":")</f>
+        <v>10</v>
+      </c>
+      <c r="C12" t="str">
+        <v xml:space="preserve"> "FG3A"</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3A</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3A VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" t="str" cm="1">
+        <f t="array" ref="B13:C13">_xlfn.TEXTSPLIT(A13, ":")</f>
+        <v>11</v>
+      </c>
+      <c r="C13" t="str">
+        <v xml:space="preserve"> "FG3_PCT"</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3_PCT</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" t="str" cm="1">
+        <f t="array" ref="B14:C14">_xlfn.TEXTSPLIT(A14, ":")</f>
+        <v>12</v>
+      </c>
+      <c r="C14" t="str">
+        <v xml:space="preserve"> "FTM"</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTM</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>FTM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15:C15">_xlfn.TEXTSPLIT(A15, ":")</f>
+        <v>13</v>
+      </c>
+      <c r="C15" t="str">
+        <v xml:space="preserve"> "FTA"</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTA</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>FTA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" t="str" cm="1">
+        <f t="array" ref="B16:C16">_xlfn.TEXTSPLIT(A16, ":")</f>
+        <v>14</v>
+      </c>
+      <c r="C16" t="str">
+        <v xml:space="preserve"> "FT_PCT"</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FT_PCT</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>FT_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" t="str" cm="1">
+        <f t="array" ref="B17:C17">_xlfn.TEXTSPLIT(A17, ":")</f>
+        <v>15</v>
+      </c>
+      <c r="C17" t="str">
+        <v xml:space="preserve"> "OREB"</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> OREB</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>OREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" t="str" cm="1">
+        <f t="array" ref="B18:C18">_xlfn.TEXTSPLIT(A18, ":")</f>
+        <v>16</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve"> "DREB"</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> DREB</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>DREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B19" t="str" cm="1">
+        <f t="array" ref="B19:C19">_xlfn.TEXTSPLIT(A19, ":")</f>
+        <v>17</v>
+      </c>
+      <c r="C19" t="str">
+        <v xml:space="preserve"> "REB"</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> REB</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>REB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" t="str" cm="1">
+        <f t="array" ref="B20:C20">_xlfn.TEXTSPLIT(A20, ":")</f>
+        <v>18</v>
+      </c>
+      <c r="C20" t="str">
+        <v xml:space="preserve"> "AST"</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> AST</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>AST VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" t="str" cm="1">
+        <f t="array" ref="B21:C21">_xlfn.TEXTSPLIT(A21, ":")</f>
+        <v>19</v>
+      </c>
+      <c r="C21" t="str">
+        <v xml:space="preserve"> "STL"</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> STL</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>STL VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B22" t="str" cm="1">
+        <f t="array" ref="B22:C22">_xlfn.TEXTSPLIT(A22, ":")</f>
+        <v>20</v>
+      </c>
+      <c r="C22" t="str">
+        <v xml:space="preserve"> "BLK"</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLK</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>BLK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" t="str" cm="1">
+        <f t="array" ref="B23:C23">_xlfn.TEXTSPLIT(A23, ":")</f>
+        <v>21</v>
+      </c>
+      <c r="C23" t="str">
+        <v xml:space="preserve"> "TO"</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TO</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>TO VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" t="str" cm="1">
+        <f t="array" ref="B24:C24">_xlfn.TEXTSPLIT(A24, ":")</f>
+        <v>22</v>
+      </c>
+      <c r="C24" t="str">
+        <v xml:space="preserve"> "PF"</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PF</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>PF VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" t="str" cm="1">
+        <f t="array" ref="B25:C25">_xlfn.TEXTSPLIT(A25, ":")</f>
+        <v>23</v>
+      </c>
+      <c r="C25" t="str">
+        <v xml:space="preserve"> "PTS"</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PTS</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>PTS VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" t="str" cm="1">
+        <f t="array" ref="B26:C26">_xlfn.TEXTSPLIT(A26, ":")</f>
+        <v>24</v>
+      </c>
+      <c r="C26" t="str">
+        <v xml:space="preserve"> "PLUS_MINUS"</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PLUS_MINUS</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>PLUS_MINUS VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4101351-5067-4F43-9C3F-A809D17FB7D0}">
+  <dimension ref="A2:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:C2">_xlfn.TEXTSPLIT(A2, ":")</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v xml:space="preserve"> "GAME_ID"</v>
+      </c>
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(C2, CHAR(34), )</f>
+        <v xml:space="preserve"> GAME_ID</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(TRIM(D2)," ",E2," ", F2, CHAR(44))</f>
+        <v>GAME_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3:C3">_xlfn.TEXTSPLIT(A3, ":")</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve"> "TEAM_ID"</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">SUBSTITUTE(C3, CHAR(34), )</f>
+        <v xml:space="preserve"> TEAM_ID</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H26" si="1">CONCATENATE(TRIM(D3)," ",E3," ", F3, CHAR(44))</f>
+        <v>TEAM_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4:C4">_xlfn.TEXTSPLIT(A4, ":")</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="str">
+        <v xml:space="preserve"> "TEAM_NAME"</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_NAME</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_NAME VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5:C5">_xlfn.TEXTSPLIT(A5, ":")</f>
+        <v>3</v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve"> "TEAM_ABBREVIATION"</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_ABBREVIATION</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_ABBREVIATION VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6:C6">_xlfn.TEXTSPLIT(A6, ":")</f>
+        <v>4</v>
+      </c>
+      <c r="C6" t="str">
+        <v xml:space="preserve"> "TEAM_CITY"</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_CITY</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_CITY VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" t="str" cm="1">
+        <f t="array" ref="B7:C7">_xlfn.TEXTSPLIT(A7, ":")</f>
+        <v>5</v>
+      </c>
+      <c r="C7" t="str">
+        <v xml:space="preserve"> "STARTERS_BENCH"</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> STARTERS_BENCH</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>STARTERS_BENCH VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" t="str" cm="1">
+        <f t="array" ref="B8:C8">_xlfn.TEXTSPLIT(A8, ":")</f>
+        <v>6</v>
+      </c>
+      <c r="C8" t="str">
+        <v xml:space="preserve"> "MIN"</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> MIN</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>MIN VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" t="str" cm="1">
+        <f t="array" ref="B9:C9">_xlfn.TEXTSPLIT(A9, ":")</f>
+        <v>7</v>
+      </c>
+      <c r="C9" t="str">
+        <v xml:space="preserve"> "FGM"</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGM</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>FGM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:C10">_xlfn.TEXTSPLIT(A10, ":")</f>
+        <v>8</v>
+      </c>
+      <c r="C10" t="str">
+        <v xml:space="preserve"> "FGA"</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGA</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>FGA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="str" cm="1">
+        <f t="array" ref="B11:C11">_xlfn.TEXTSPLIT(A11, ":")</f>
+        <v>9</v>
+      </c>
+      <c r="C11" t="str">
+        <v xml:space="preserve"> "FG_PCT"</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG_PCT</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>FG_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" t="str" cm="1">
+        <f t="array" ref="B12:C12">_xlfn.TEXTSPLIT(A12, ":")</f>
+        <v>10</v>
+      </c>
+      <c r="C12" t="str">
+        <v xml:space="preserve"> "FG3M"</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3M</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3M VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" t="str" cm="1">
+        <f t="array" ref="B13:C13">_xlfn.TEXTSPLIT(A13, ":")</f>
+        <v>11</v>
+      </c>
+      <c r="C13" t="str">
+        <v xml:space="preserve"> "FG3A"</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3A</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3A VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" t="str" cm="1">
+        <f t="array" ref="B14:C14">_xlfn.TEXTSPLIT(A14, ":")</f>
+        <v>12</v>
+      </c>
+      <c r="C14" t="str">
+        <v xml:space="preserve"> "FG3_PCT"</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3_PCT</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15:C15">_xlfn.TEXTSPLIT(A15, ":")</f>
+        <v>13</v>
+      </c>
+      <c r="C15" t="str">
+        <v xml:space="preserve"> "FTM"</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTM</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>FTM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" t="str" cm="1">
+        <f t="array" ref="B16:C16">_xlfn.TEXTSPLIT(A16, ":")</f>
+        <v>14</v>
+      </c>
+      <c r="C16" t="str">
+        <v xml:space="preserve"> "FTA"</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTA</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>FTA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" t="str" cm="1">
+        <f t="array" ref="B17:C17">_xlfn.TEXTSPLIT(A17, ":")</f>
+        <v>15</v>
+      </c>
+      <c r="C17" t="str">
+        <v xml:space="preserve"> "FT_PCT"</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FT_PCT</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>FT_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" t="str" cm="1">
+        <f t="array" ref="B18:C18">_xlfn.TEXTSPLIT(A18, ":")</f>
+        <v>16</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve"> "OREB"</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> OREB</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>OREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" t="str" cm="1">
+        <f t="array" ref="B19:C19">_xlfn.TEXTSPLIT(A19, ":")</f>
+        <v>17</v>
+      </c>
+      <c r="C19" t="str">
+        <v xml:space="preserve"> "DREB"</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> DREB</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>DREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" t="str" cm="1">
+        <f t="array" ref="B20:C20">_xlfn.TEXTSPLIT(A20, ":")</f>
+        <v>18</v>
+      </c>
+      <c r="C20" t="str">
+        <v xml:space="preserve"> "REB"</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> REB</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>REB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" t="str" cm="1">
+        <f t="array" ref="B21:C21">_xlfn.TEXTSPLIT(A21, ":")</f>
+        <v>19</v>
+      </c>
+      <c r="C21" t="str">
+        <v xml:space="preserve"> "AST"</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> AST</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>AST VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" t="str" cm="1">
+        <f t="array" ref="B22:C22">_xlfn.TEXTSPLIT(A22, ":")</f>
+        <v>20</v>
+      </c>
+      <c r="C22" t="str">
+        <v xml:space="preserve"> "STL"</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> STL</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>STL VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" t="str" cm="1">
+        <f t="array" ref="B23:C23">_xlfn.TEXTSPLIT(A23, ":")</f>
+        <v>21</v>
+      </c>
+      <c r="C23" t="str">
+        <v xml:space="preserve"> "BLK"</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLK</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>BLK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" t="str" cm="1">
+        <f t="array" ref="B24:C24">_xlfn.TEXTSPLIT(A24, ":")</f>
+        <v>22</v>
+      </c>
+      <c r="C24" t="str">
+        <v xml:space="preserve"> "TO"</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TO</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>TO VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" t="str" cm="1">
+        <f t="array" ref="B25:C25">_xlfn.TEXTSPLIT(A25, ":")</f>
+        <v>23</v>
+      </c>
+      <c r="C25" t="str">
+        <v xml:space="preserve"> "PF"</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PF</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>PF VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" t="str" cm="1">
+        <f t="array" ref="B26:C26">_xlfn.TEXTSPLIT(A26, ":")</f>
+        <v>24</v>
+      </c>
+      <c r="C26" t="str">
+        <v xml:space="preserve"> "PTS"</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PTS</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>PTS VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E5"/>
@@ -3369,7 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -3951,17 +5503,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F8D3D1-9A33-4874-9CEA-68E5282DA8C2}">
   <dimension ref="A2:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
@@ -3986,8 +5540,8 @@
         <v>17</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE(D2," ",E2," ", F2, CHAR(44))</f>
-        <v xml:space="preserve"> SEASON_YEAR VARCHAR(45) NOT NULL,</v>
+        <f>CONCATENATE(TRIM(D2)," ",E2," ", F2, CHAR(44))</f>
+        <v>SEASON_YEAR VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4012,8 +5566,8 @@
         <v>17</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H58" si="1">CONCATENATE(D3," ",E3," ", F3, CHAR(44))</f>
-        <v xml:space="preserve"> TEAM_ID VARCHAR(45) NOT NULL,</v>
+        <f t="shared" ref="H3:H58" si="1">CONCATENATE(TRIM(D3)," ",E3," ", F3, CHAR(44))</f>
+        <v>TEAM_ID VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4039,7 +5593,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TEAM_ABBREVIATION VARCHAR(45) NOT NULL,</v>
+        <v>TEAM_ABBREVIATION VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4065,7 +5619,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TEAM_NAME VARCHAR(45) NOT NULL,</v>
+        <v>TEAM_NAME VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4091,7 +5645,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> GAME_ID VARCHAR(45) NOT NULL,</v>
+        <v>GAME_ID VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4117,7 +5671,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> GAME_DATE VARCHAR(45) NOT NULL,</v>
+        <v>GAME_DATE VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4143,7 +5697,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> MATCHUP VARCHAR(45) NOT NULL,</v>
+        <v>MATCHUP VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -4169,7 +5723,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> WL VARCHAR(45) NOT NULL,</v>
+        <v>WL VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4195,7 +5749,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> MIN VARCHAR(45) NOT NULL,</v>
+        <v>MIN VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4221,7 +5775,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FGM VARCHAR(45) NOT NULL,</v>
+        <v>FGM VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4247,7 +5801,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FGA VARCHAR(45) NOT NULL,</v>
+        <v>FGA VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4273,7 +5827,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG_PCT VARCHAR(45) NOT NULL,</v>
+        <v>FG_PCT VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4299,7 +5853,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG3M VARCHAR(45) NOT NULL,</v>
+        <v>FG3M VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4325,7 +5879,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG3A VARCHAR(45) NOT NULL,</v>
+        <v>FG3A VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -4351,7 +5905,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG3_PCT VARCHAR(45) NOT NULL,</v>
+        <v>FG3_PCT VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -4377,7 +5931,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FTM VARCHAR(45) NOT NULL,</v>
+        <v>FTM VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -4403,7 +5957,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FTA VARCHAR(45) NOT NULL,</v>
+        <v>FTA VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -4429,7 +5983,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FT_PCT VARCHAR(45) NOT NULL,</v>
+        <v>FT_PCT VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -4455,7 +6009,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> OREB VARCHAR(45) NOT NULL,</v>
+        <v>OREB VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -4481,7 +6035,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> DREB VARCHAR(45) NOT NULL,</v>
+        <v>DREB VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -4507,7 +6061,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> REB VARCHAR(45) NOT NULL,</v>
+        <v>REB VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -4533,7 +6087,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> AST VARCHAR(45) NOT NULL,</v>
+        <v>AST VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -4559,7 +6113,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TOV VARCHAR(45) NOT NULL,</v>
+        <v>TOV VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -4585,7 +6139,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> STL VARCHAR(45) NOT NULL,</v>
+        <v>STL VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -4611,7 +6165,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> BLK VARCHAR(45) NOT NULL,</v>
+        <v>BLK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4637,7 +6191,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> BLKA VARCHAR(45) NOT NULL,</v>
+        <v>BLKA VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -4663,7 +6217,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PF VARCHAR(45) NOT NULL,</v>
+        <v>PF VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -4689,7 +6243,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PFD VARCHAR(45) NOT NULL,</v>
+        <v>PFD VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -4715,7 +6269,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PTS VARCHAR(45) NOT NULL,</v>
+        <v>PTS VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -4741,7 +6295,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PLUS_MINUS VARCHAR(45) NOT NULL,</v>
+        <v>PLUS_MINUS VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -4767,7 +6321,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> GP_RANK VARCHAR(45) NOT NULL,</v>
+        <v>GP_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -4793,7 +6347,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> W_RANK VARCHAR(45) NOT NULL,</v>
+        <v>W_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -4819,7 +6373,7 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> L_RANK VARCHAR(45) NOT NULL,</v>
+        <v>L_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -4845,7 +6399,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> W_PCT_RANK VARCHAR(45) NOT NULL,</v>
+        <v>W_PCT_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -4871,7 +6425,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> MIN_RANK VARCHAR(45) NOT NULL,</v>
+        <v>MIN_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -4897,7 +6451,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FGM_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FGM_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -4923,7 +6477,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FGA_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FGA_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -4949,7 +6503,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG_PCT_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FG_PCT_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -4975,7 +6529,7 @@
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG3M_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FG3M_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -5001,7 +6555,7 @@
       </c>
       <c r="H41" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG3A_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FG3A_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -5027,7 +6581,7 @@
       </c>
       <c r="H42" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FG3_PCT_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FG3_PCT_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -5053,7 +6607,7 @@
       </c>
       <c r="H43" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FTM_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FTM_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -5079,7 +6633,7 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FTA_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FTA_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -5105,7 +6659,7 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> FT_PCT_RANK VARCHAR(45) NOT NULL,</v>
+        <v>FT_PCT_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -5131,7 +6685,7 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> OREB_RANK VARCHAR(45) NOT NULL,</v>
+        <v>OREB_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -5157,7 +6711,7 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> DREB_RANK VARCHAR(45) NOT NULL,</v>
+        <v>DREB_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -5183,7 +6737,7 @@
       </c>
       <c r="H48" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> REB_RANK VARCHAR(45) NOT NULL,</v>
+        <v>REB_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -5209,7 +6763,7 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> AST_RANK VARCHAR(45) NOT NULL,</v>
+        <v>AST_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -5235,7 +6789,7 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TOV_RANK VARCHAR(45) NOT NULL,</v>
+        <v>TOV_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -5261,7 +6815,7 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> STL_RANK VARCHAR(45) NOT NULL,</v>
+        <v>STL_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -5287,7 +6841,7 @@
       </c>
       <c r="H52" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> BLK_RANK VARCHAR(45) NOT NULL,</v>
+        <v>BLK_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -5313,7 +6867,7 @@
       </c>
       <c r="H53" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> BLKA_RANK VARCHAR(45) NOT NULL,</v>
+        <v>BLKA_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -5339,7 +6893,7 @@
       </c>
       <c r="H54" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PF_RANK VARCHAR(45) NOT NULL,</v>
+        <v>PF_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -5365,7 +6919,7 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PFD_RANK VARCHAR(45) NOT NULL,</v>
+        <v>PFD_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -5391,7 +6945,7 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PTS_RANK VARCHAR(45) NOT NULL,</v>
+        <v>PTS_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -5417,7 +6971,7 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> PLUS_MINUS_RANK VARCHAR(45) NOT NULL,</v>
+        <v>PLUS_MINUS_RANK VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -5443,7 +6997,786 @@
       </c>
       <c r="H58" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> AVAILABLE_FLAG VARCHAR(45) NOT NULL,</v>
+        <v>AVAILABLE_FLAG VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF5ED38-B5C0-401F-BC6D-E31C3D4A7F76}">
+  <dimension ref="A2:H30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:C2">_xlfn.TEXTSPLIT(A2, ":")</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v xml:space="preserve"> "GAME_ID"</v>
+      </c>
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(C2, CHAR(34), )</f>
+        <v xml:space="preserve"> GAME_ID</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(TRIM(D2)," ",E2," ", F2, CHAR(44))</f>
+        <v>GAME_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3:C3">_xlfn.TEXTSPLIT(A3, ":")</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve"> "TEAM_ID"</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D31" si="0">SUBSTITUTE(C3, CHAR(34), )</f>
+        <v xml:space="preserve"> TEAM_ID</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H30" si="1">CONCATENATE(TRIM(D3)," ",E3," ", F3, CHAR(44))</f>
+        <v>TEAM_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4:C4">_xlfn.TEXTSPLIT(A4, ":")</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="str">
+        <v xml:space="preserve"> "TEAM_ABBREVIATION"</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_ABBREVIATION</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_ABBREVIATION VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5:C5">_xlfn.TEXTSPLIT(A5, ":")</f>
+        <v>3</v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve"> "TEAM_CITY"</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TEAM_CITY</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>TEAM_CITY VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6:C6">_xlfn.TEXTSPLIT(A6, ":")</f>
+        <v>4</v>
+      </c>
+      <c r="C6" t="str">
+        <v xml:space="preserve"> "PLAYER_ID"</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PLAYER_ID</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>PLAYER_ID VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="str" cm="1">
+        <f t="array" ref="B7:C7">_xlfn.TEXTSPLIT(A7, ":")</f>
+        <v>5</v>
+      </c>
+      <c r="C7" t="str">
+        <v xml:space="preserve"> "PLAYER_NAME"</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PLAYER_NAME</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>PLAYER_NAME VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" t="str" cm="1">
+        <f t="array" ref="B8:C8">_xlfn.TEXTSPLIT(A8, ":")</f>
+        <v>6</v>
+      </c>
+      <c r="C8" t="str">
+        <v xml:space="preserve"> "NICKNAME"</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> NICKNAME</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>NICKNAME VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="str" cm="1">
+        <f t="array" ref="B9:C9">_xlfn.TEXTSPLIT(A9, ":")</f>
+        <v>7</v>
+      </c>
+      <c r="C9" t="str">
+        <v xml:space="preserve"> "START_POSITION"</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> START_POSITION</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>START_POSITION VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:C10">_xlfn.TEXTSPLIT(A10, ":")</f>
+        <v>8</v>
+      </c>
+      <c r="C10" t="str">
+        <v xml:space="preserve"> "COMMENT"</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> COMMENT</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>COMMENT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" t="str" cm="1">
+        <f t="array" ref="B11:C11">_xlfn.TEXTSPLIT(A11, ":")</f>
+        <v>9</v>
+      </c>
+      <c r="C11" t="str">
+        <v xml:space="preserve"> "MIN"</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> MIN</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>MIN VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" t="str" cm="1">
+        <f t="array" ref="B12:C12">_xlfn.TEXTSPLIT(A12, ":")</f>
+        <v>10</v>
+      </c>
+      <c r="C12" t="str">
+        <v xml:space="preserve"> "FGM"</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGM</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>FGM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" t="str" cm="1">
+        <f t="array" ref="B13:C13">_xlfn.TEXTSPLIT(A13, ":")</f>
+        <v>11</v>
+      </c>
+      <c r="C13" t="str">
+        <v xml:space="preserve"> "FGA"</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FGA</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>FGA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" t="str" cm="1">
+        <f t="array" ref="B14:C14">_xlfn.TEXTSPLIT(A14, ":")</f>
+        <v>12</v>
+      </c>
+      <c r="C14" t="str">
+        <v xml:space="preserve"> "FG_PCT"</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG_PCT</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>FG_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15:C15">_xlfn.TEXTSPLIT(A15, ":")</f>
+        <v>13</v>
+      </c>
+      <c r="C15" t="str">
+        <v xml:space="preserve"> "FG3M"</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3M</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3M VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" t="str" cm="1">
+        <f t="array" ref="B16:C16">_xlfn.TEXTSPLIT(A16, ":")</f>
+        <v>14</v>
+      </c>
+      <c r="C16" t="str">
+        <v xml:space="preserve"> "FG3A"</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3A</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3A VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" t="str" cm="1">
+        <f t="array" ref="B17:C17">_xlfn.TEXTSPLIT(A17, ":")</f>
+        <v>15</v>
+      </c>
+      <c r="C17" t="str">
+        <v xml:space="preserve"> "FG3_PCT"</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FG3_PCT</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>FG3_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" t="str" cm="1">
+        <f t="array" ref="B18:C18">_xlfn.TEXTSPLIT(A18, ":")</f>
+        <v>16</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve"> "FTM"</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTM</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>FTM VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" t="str" cm="1">
+        <f t="array" ref="B19:C19">_xlfn.TEXTSPLIT(A19, ":")</f>
+        <v>17</v>
+      </c>
+      <c r="C19" t="str">
+        <v xml:space="preserve"> "FTA"</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FTA</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>FTA VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" t="str" cm="1">
+        <f t="array" ref="B20:C20">_xlfn.TEXTSPLIT(A20, ":")</f>
+        <v>18</v>
+      </c>
+      <c r="C20" t="str">
+        <v xml:space="preserve"> "FT_PCT"</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> FT_PCT</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>FT_PCT VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="str" cm="1">
+        <f t="array" ref="B21:C21">_xlfn.TEXTSPLIT(A21, ":")</f>
+        <v>19</v>
+      </c>
+      <c r="C21" t="str">
+        <v xml:space="preserve"> "OREB"</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> OREB</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>OREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" t="str" cm="1">
+        <f t="array" ref="B22:C22">_xlfn.TEXTSPLIT(A22, ":")</f>
+        <v>20</v>
+      </c>
+      <c r="C22" t="str">
+        <v xml:space="preserve"> "DREB"</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> DREB</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>DREB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" t="str" cm="1">
+        <f t="array" ref="B23:C23">_xlfn.TEXTSPLIT(A23, ":")</f>
+        <v>21</v>
+      </c>
+      <c r="C23" t="str">
+        <v xml:space="preserve"> "REB"</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> REB</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>REB VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" t="str" cm="1">
+        <f t="array" ref="B24:C24">_xlfn.TEXTSPLIT(A24, ":")</f>
+        <v>22</v>
+      </c>
+      <c r="C24" t="str">
+        <v xml:space="preserve"> "AST"</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> AST</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>AST VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" t="str" cm="1">
+        <f t="array" ref="B25:C25">_xlfn.TEXTSPLIT(A25, ":")</f>
+        <v>23</v>
+      </c>
+      <c r="C25" t="str">
+        <v xml:space="preserve"> "STL"</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> STL</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>STL VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="str" cm="1">
+        <f t="array" ref="B26:C26">_xlfn.TEXTSPLIT(A26, ":")</f>
+        <v>24</v>
+      </c>
+      <c r="C26" t="str">
+        <v xml:space="preserve"> "BLK"</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> BLK</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>BLK VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27" t="str" cm="1">
+        <f t="array" ref="B27:C27">_xlfn.TEXTSPLIT(A27, ":")</f>
+        <v>25</v>
+      </c>
+      <c r="C27" t="str">
+        <v xml:space="preserve"> "TO"</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> TO</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>TO VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="str" cm="1">
+        <f t="array" ref="B28:C28">_xlfn.TEXTSPLIT(A28, ":")</f>
+        <v>26</v>
+      </c>
+      <c r="C28" t="str">
+        <v xml:space="preserve"> "PF"</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PF</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>PF VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" t="str" cm="1">
+        <f t="array" ref="B29:C29">_xlfn.TEXTSPLIT(A29, ":")</f>
+        <v>27</v>
+      </c>
+      <c r="C29" t="str">
+        <v xml:space="preserve"> "PTS"</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PTS</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>PTS VARCHAR(45) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" t="str" cm="1">
+        <f t="array" ref="B30:C30">_xlfn.TEXTSPLIT(A30, ":")</f>
+        <v>28</v>
+      </c>
+      <c r="C30" t="str">
+        <v xml:space="preserve"> "PLUS_MINUS"</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> PLUS_MINUS</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>PLUS_MINUS VARCHAR(45) NOT NULL,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>